<commit_message>
Unit testing  initial report for Host Login
</commit_message>
<xml_diff>
--- a/Host .xlsx
+++ b/Host .xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="82">
   <si>
     <t>Test case number</t>
   </si>
@@ -201,9 +201,6 @@
     <t>Create event</t>
   </si>
   <si>
-    <t>a.reate a new event by adding event name ,Date and time</t>
-  </si>
-  <si>
     <t>b.Host must be able to see the list of guards .</t>
   </si>
   <si>
@@ -223,14 +220,73 @@
   </si>
   <si>
     <t xml:space="preserve">c. If Host click on edit option </t>
+  </si>
+  <si>
+    <t>a.Create a new event by adding event name ,Date and time</t>
+  </si>
+  <si>
+    <t>Create a new event by adding event name ,Date and time</t>
+  </si>
+  <si>
+    <t>Able to see list of guards</t>
+  </si>
+  <si>
+    <t>Images of the profiles must be of same size</t>
+  </si>
+  <si>
+    <t>Images must be consistent in size</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Alignment of the elements in the page</t>
+  </si>
+  <si>
+    <t>Alignemnt should be proper</t>
+  </si>
+  <si>
+    <t>Reset button clear all the fields in the create events page.</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Members</t>
+  </si>
+  <si>
+    <t>Display the list of all members</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Edit the the customer</t>
+  </si>
+  <si>
+    <t>Edit the customer</t>
+  </si>
+  <si>
+    <t>Delete the particular customer</t>
+  </si>
+  <si>
+    <t>delete particular customer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -264,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -273,6 +329,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -788,10 +846,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,8 +857,8 @@
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" customWidth="1"/>
     <col min="3" max="3" width="40.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -813,10 +871,10 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -861,54 +919,171 @@
       <c r="C9" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>57</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="C18" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="3" t="s">
+    </row>
+    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C19" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="3:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C17" s="3" t="s">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="3" t="s">
-        <v>65</v>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>